<commit_message>
feat[logging]: add base logger and replace prints in data_loader + status recap
</commit_message>
<xml_diff>
--- a/data/Fissures/Fissure_2.xlsx
+++ b/data/Fissures/Fissure_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\PycharmProjects\Fissure\data\Fissures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D501B7D2-8110-48AD-AB50-6179707B5DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E7332E-58C8-4AF0-B8A7-B7B5261AAF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ81"/>
+  <dimension ref="A1:AMJ82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -2052,12 +2052,31 @@
         <v>89.93</v>
       </c>
       <c r="D81" s="8">
-        <f t="shared" ref="D81" si="20">B81-B80</f>
+        <f t="shared" ref="D81:D82" si="20">B81-B80</f>
         <v>3.0000000000001137E-2</v>
       </c>
       <c r="E81" s="8">
-        <f t="shared" ref="E81" si="21">C81-C80</f>
+        <f t="shared" ref="E81:E82" si="21">C81-C80</f>
         <v>-0.31999999999999318</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="3">
+        <v>45830</v>
+      </c>
+      <c r="B82" s="6">
+        <v>30.26</v>
+      </c>
+      <c r="C82" s="6">
+        <v>89.5</v>
+      </c>
+      <c r="D82" s="8">
+        <f t="shared" si="20"/>
+        <v>5.0000000000000711E-2</v>
+      </c>
+      <c r="E82" s="8">
+        <f t="shared" si="21"/>
+        <v>-0.43000000000000682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>